<commit_message>
feat: add new values to lookup tables and correct spelling
SVC-1467
</commit_message>
<xml_diff>
--- a/annex-2-3/mappings6.0/Buildings/2D/Unterlagen/TabellenBuildingNature/AX_Bauwerksfunktion_BauwerkImGewaesserbereich.xlsx
+++ b/annex-2-3/mappings6.0/Buildings/2D/Unterlagen/TabellenBuildingNature/AX_Bauwerksfunktion_BauwerkImGewaesserbereich.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johanna Ott\Box Sync\staff\Projects\2017-10 AdV Umsetzung Annex II und III\Alignments\BU\2D\TabellenBuildingNature\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johanna Ott\git\adv-inspire-alignments\annex-2-3\mappings6.0\Buildings\2D\Unterlagen\TabellenBuildingNature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D05A201F-7A20-496B-ADC4-FE90433FA5F1}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D8F9FE-D896-4CC2-8EE2-D0995A2AFABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="5670" xr2:uid="{7191D6A3-C2E8-4C58-A0DE-E66D09F315E3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7191D6A3-C2E8-4C58-A0DE-E66D09F315E3}"/>
   </bookViews>
   <sheets>
     <sheet name="AX_Gebaeudefunktion" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>Wert</t>
   </si>
@@ -67,6 +67,15 @@
   </si>
   <si>
     <t>http://inspire.ec.europa.eu/codelist/BuildingNatureValue/dam</t>
+  </si>
+  <si>
+    <t>Wassertunnel, Wasserstollen, Druckstollen</t>
+  </si>
+  <si>
+    <t>http://inspire.ec.europa.eu/codelist/BuildingNatureValue/caveBuilding</t>
+  </si>
+  <si>
+    <t>Verschlussbauwerk</t>
   </si>
 </sst>
 </file>
@@ -119,31 +128,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -159,7 +155,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -455,13 +451,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C1D5605-B657-42F0-8600-405EFB21280B}">
-  <dimension ref="A1:E233"/>
+  <dimension ref="A1:E235"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="68.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="67.85546875" bestFit="1" customWidth="1"/>
@@ -486,44 +482,46 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2">
-        <v>2030</v>
+      <c r="A2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="4">
+        <v>2023</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>13</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2">
-        <v>2040</v>
-      </c>
-      <c r="C3" s="4" t="s">
+        <v>2030</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2">
-        <v>2050</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>12</v>
+        <v>2040</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2">
-        <v>2060</v>
+        <v>2050</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>12</v>
@@ -531,10 +529,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="2">
-        <v>2070</v>
+        <v>2060</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>12</v>
@@ -542,10 +540,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2">
-        <v>2080</v>
+        <v>2070</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>12</v>
@@ -553,264 +551,278 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B8" s="2">
-        <v>2090</v>
+        <v>2080</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="8"/>
+      <c r="A9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="2">
+        <v>2085</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="5"/>
+      <c r="A10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="2">
+        <v>2090</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
-      <c r="C11" s="5"/>
+      <c r="C11" s="3"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="15"/>
+      <c r="C12" s="3"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="15"/>
+      <c r="C13" s="3"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="15"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="15"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="11"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="11"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="9"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="9"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="9"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="9"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="9"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
-      <c r="C23" s="5"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
-      <c r="C24" s="5"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
-      <c r="C25" s="5"/>
+      <c r="C25" s="3"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
-      <c r="C26" s="5"/>
+      <c r="C26" s="3"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="16"/>
+      <c r="C27" s="3"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
-      <c r="C28" s="16"/>
+      <c r="C28" s="3"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
-      <c r="C29" s="17"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
-      <c r="C30" s="16"/>
+      <c r="C30" s="3"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
-      <c r="C31" s="17"/>
+      <c r="C31" s="3"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
-      <c r="C32" s="17"/>
+      <c r="C32" s="3"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
-      <c r="C33" s="17"/>
+      <c r="C33" s="3"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
-      <c r="C34" s="17"/>
+      <c r="C34" s="3"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
-      <c r="C35" s="17"/>
+      <c r="C35" s="3"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
-      <c r="C36" s="17"/>
+      <c r="C36" s="3"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
-      <c r="C37" s="17"/>
+      <c r="C37" s="3"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
-      <c r="C38" s="17"/>
+      <c r="C38" s="3"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
-      <c r="C39" s="17"/>
+      <c r="C39" s="3"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
-      <c r="C40" s="17"/>
+      <c r="C40" s="3"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
-      <c r="C41" s="17"/>
+      <c r="C41" s="3"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
-      <c r="C42" s="17"/>
+      <c r="C42" s="3"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
-      <c r="C43" s="17"/>
+      <c r="C43" s="3"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
-      <c r="C44" s="17"/>
+      <c r="C44" s="3"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
-      <c r="C45" s="17"/>
+      <c r="C45" s="3"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
-      <c r="C46" s="17"/>
+      <c r="C46" s="3"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
-      <c r="C47" s="17"/>
+      <c r="C47" s="3"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
-      <c r="C48" s="17"/>
+      <c r="C48" s="3"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
-      <c r="C49" s="17"/>
+      <c r="C49" s="3"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
-      <c r="C50" s="17"/>
+      <c r="C50" s="3"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
-      <c r="C51" s="17"/>
+      <c r="C51" s="3"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
-      <c r="C52" s="17"/>
+      <c r="C52" s="3"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
-      <c r="C53" s="17"/>
+      <c r="C53" s="3"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
-      <c r="C54" s="13"/>
+      <c r="C54" s="3"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
+      <c r="C55" s="3"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
+      <c r="C56" s="3"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
@@ -844,86 +856,86 @@
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
-      <c r="C80" s="6"/>
-      <c r="D80" s="17"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
-      <c r="C81" s="6"/>
-      <c r="D81" s="14"/>
-      <c r="E81" s="17"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
+      <c r="C82" s="3"/>
+      <c r="D82" s="3"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
+      <c r="E83" s="3"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
@@ -1128,505 +1140,516 @@
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="2"/>
       <c r="B134" s="2"/>
-      <c r="C134" s="10"/>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="2"/>
       <c r="B135" s="2"/>
-      <c r="C135" s="10"/>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="2"/>
       <c r="B136" s="2"/>
-      <c r="C136" s="10"/>
+      <c r="C136" s="3"/>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="2"/>
       <c r="B137" s="2"/>
-      <c r="C137" s="10"/>
+      <c r="C137" s="3"/>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="2"/>
       <c r="B138" s="2"/>
-      <c r="C138" s="10"/>
+      <c r="C138" s="3"/>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="2"/>
       <c r="B139" s="2"/>
-      <c r="C139" s="10"/>
+      <c r="C139" s="3"/>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="2"/>
       <c r="B140" s="2"/>
-      <c r="C140" s="10"/>
+      <c r="C140" s="3"/>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="2"/>
       <c r="B141" s="2"/>
-      <c r="C141" s="10"/>
+      <c r="C141" s="3"/>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="2"/>
       <c r="B142" s="2"/>
-      <c r="C142" s="10"/>
+      <c r="C142" s="3"/>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="2"/>
       <c r="B143" s="2"/>
-      <c r="C143" s="10"/>
+      <c r="C143" s="3"/>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="2"/>
       <c r="B144" s="2"/>
-      <c r="C144" s="10"/>
+      <c r="C144" s="3"/>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="2"/>
       <c r="B145" s="2"/>
-      <c r="C145" s="10"/>
+      <c r="C145" s="3"/>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="2"/>
       <c r="B146" s="2"/>
-      <c r="C146" s="10"/>
+      <c r="C146" s="3"/>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="2"/>
       <c r="B147" s="2"/>
-      <c r="C147" s="10"/>
+      <c r="C147" s="3"/>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="2"/>
       <c r="B148" s="2"/>
-      <c r="C148" s="17"/>
+      <c r="C148" s="3"/>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="2"/>
       <c r="B149" s="2"/>
-      <c r="C149" s="17"/>
+      <c r="C149" s="3"/>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="2"/>
       <c r="B150" s="2"/>
-      <c r="C150" s="17"/>
+      <c r="C150" s="3"/>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="2"/>
       <c r="B151" s="2"/>
-      <c r="C151" s="17"/>
+      <c r="C151" s="3"/>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="2"/>
       <c r="B152" s="2"/>
-      <c r="C152" s="17"/>
+      <c r="C152" s="3"/>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="2"/>
       <c r="B153" s="2"/>
-      <c r="C153" s="17"/>
+      <c r="C153" s="3"/>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="2"/>
       <c r="B154" s="2"/>
-      <c r="C154" s="17"/>
+      <c r="C154" s="3"/>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="2"/>
       <c r="B155" s="2"/>
-      <c r="C155" s="17"/>
+      <c r="C155" s="3"/>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="2"/>
       <c r="B156" s="2"/>
-      <c r="C156" s="17"/>
+      <c r="C156" s="3"/>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="2"/>
       <c r="B157" s="2"/>
-      <c r="C157" s="17"/>
+      <c r="C157" s="3"/>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="2"/>
       <c r="B158" s="2"/>
-      <c r="C158" s="17"/>
+      <c r="C158" s="3"/>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="2"/>
       <c r="B159" s="2"/>
-      <c r="C159" s="17"/>
+      <c r="C159" s="3"/>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="2"/>
       <c r="B160" s="2"/>
-      <c r="C160" s="17"/>
+      <c r="C160" s="3"/>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="2"/>
       <c r="B161" s="2"/>
-      <c r="C161" s="17"/>
+      <c r="C161" s="3"/>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="2"/>
       <c r="B162" s="2"/>
-      <c r="C162" s="17"/>
+      <c r="C162" s="3"/>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="2"/>
       <c r="B163" s="2"/>
-      <c r="C163" s="17"/>
+      <c r="C163" s="3"/>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="2"/>
       <c r="B164" s="2"/>
-      <c r="C164" s="17"/>
+      <c r="C164" s="3"/>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="2"/>
       <c r="B165" s="2"/>
-      <c r="C165" s="17"/>
+      <c r="C165" s="3"/>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="2"/>
       <c r="B166" s="2"/>
-      <c r="C166" s="17"/>
+      <c r="C166" s="3"/>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="2"/>
       <c r="B167" s="2"/>
-      <c r="C167" s="17"/>
+      <c r="C167" s="3"/>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="2"/>
       <c r="B168" s="2"/>
-      <c r="C168" s="17"/>
+      <c r="C168" s="3"/>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="2"/>
       <c r="B169" s="2"/>
-      <c r="C169" s="17"/>
+      <c r="C169" s="3"/>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="2"/>
       <c r="B170" s="2"/>
-      <c r="C170" s="17"/>
+      <c r="C170" s="3"/>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="2"/>
       <c r="B171" s="2"/>
-      <c r="C171" s="17"/>
+      <c r="C171" s="3"/>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="2"/>
       <c r="B172" s="2"/>
-      <c r="C172" s="17"/>
+      <c r="C172" s="3"/>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="2"/>
       <c r="B173" s="2"/>
-      <c r="C173" s="17"/>
+      <c r="C173" s="3"/>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="2"/>
       <c r="B174" s="2"/>
-      <c r="C174" s="17"/>
+      <c r="C174" s="3"/>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="2"/>
       <c r="B175" s="2"/>
-      <c r="C175" s="17"/>
+      <c r="C175" s="3"/>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="2"/>
       <c r="B176" s="2"/>
-      <c r="C176" s="17"/>
+      <c r="C176" s="3"/>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="2"/>
       <c r="B177" s="2"/>
-      <c r="C177" s="17"/>
+      <c r="C177" s="3"/>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" s="2"/>
       <c r="B178" s="2"/>
-      <c r="C178" s="17"/>
+      <c r="C178" s="3"/>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" s="2"/>
       <c r="B179" s="2"/>
-      <c r="C179" s="17"/>
+      <c r="C179" s="3"/>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="2"/>
       <c r="B180" s="2"/>
-      <c r="C180" s="17"/>
+      <c r="C180" s="3"/>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" s="2"/>
       <c r="B181" s="2"/>
-      <c r="C181" s="17"/>
+      <c r="C181" s="3"/>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" s="2"/>
       <c r="B182" s="2"/>
-      <c r="C182" s="17"/>
+      <c r="C182" s="3"/>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" s="2"/>
       <c r="B183" s="2"/>
-      <c r="C183" s="17"/>
+      <c r="C183" s="3"/>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" s="2"/>
       <c r="B184" s="2"/>
-      <c r="C184" s="17"/>
+      <c r="C184" s="3"/>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" s="2"/>
       <c r="B185" s="2"/>
-      <c r="C185" s="17"/>
+      <c r="C185" s="3"/>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" s="2"/>
       <c r="B186" s="2"/>
-      <c r="C186" s="17"/>
+      <c r="C186" s="3"/>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" s="2"/>
       <c r="B187" s="2"/>
-      <c r="C187" s="17"/>
+      <c r="C187" s="3"/>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" s="2"/>
       <c r="B188" s="2"/>
-      <c r="C188" s="17"/>
+      <c r="C188" s="3"/>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" s="2"/>
       <c r="B189" s="2"/>
-      <c r="C189" s="17"/>
+      <c r="C189" s="3"/>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" s="2"/>
       <c r="B190" s="2"/>
-      <c r="C190" s="17"/>
+      <c r="C190" s="3"/>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" s="2"/>
       <c r="B191" s="2"/>
-      <c r="C191" s="17"/>
+      <c r="C191" s="3"/>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" s="2"/>
       <c r="B192" s="2"/>
-      <c r="C192" s="17"/>
+      <c r="C192" s="3"/>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" s="2"/>
       <c r="B193" s="2"/>
-      <c r="C193" s="17"/>
+      <c r="C193" s="3"/>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" s="2"/>
       <c r="B194" s="2"/>
-      <c r="C194" s="17"/>
+      <c r="C194" s="3"/>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" s="2"/>
       <c r="B195" s="2"/>
-      <c r="C195" s="17"/>
+      <c r="C195" s="3"/>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="2"/>
       <c r="B196" s="2"/>
-      <c r="C196" s="17"/>
+      <c r="C196" s="3"/>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" s="2"/>
       <c r="B197" s="2"/>
-      <c r="C197" s="17"/>
+      <c r="C197" s="3"/>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" s="2"/>
       <c r="B198" s="2"/>
-      <c r="C198" s="17"/>
+      <c r="C198" s="3"/>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" s="2"/>
       <c r="B199" s="2"/>
-      <c r="C199" s="17"/>
+      <c r="C199" s="3"/>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" s="2"/>
       <c r="B200" s="2"/>
-      <c r="C200" s="17"/>
+      <c r="C200" s="3"/>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" s="2"/>
       <c r="B201" s="2"/>
-      <c r="C201" s="17"/>
+      <c r="C201" s="3"/>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" s="2"/>
       <c r="B202" s="2"/>
-      <c r="C202" s="17"/>
+      <c r="C202" s="3"/>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" s="2"/>
       <c r="B203" s="2"/>
-      <c r="C203" s="17"/>
+      <c r="C203" s="3"/>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" s="2"/>
       <c r="B204" s="2"/>
-      <c r="C204" s="17"/>
+      <c r="C204" s="3"/>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" s="2"/>
       <c r="B205" s="2"/>
-      <c r="C205" s="17"/>
+      <c r="C205" s="3"/>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" s="2"/>
       <c r="B206" s="2"/>
-      <c r="C206" s="17"/>
+      <c r="C206" s="3"/>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" s="2"/>
       <c r="B207" s="2"/>
-      <c r="C207" s="17"/>
+      <c r="C207" s="3"/>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" s="2"/>
       <c r="B208" s="2"/>
-      <c r="C208" s="17"/>
+      <c r="C208" s="3"/>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" s="2"/>
       <c r="B209" s="2"/>
-      <c r="C209" s="7"/>
-      <c r="D209" s="17"/>
+      <c r="C209" s="3"/>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" s="2"/>
       <c r="B210" s="2"/>
-      <c r="C210" s="17"/>
+      <c r="C210" s="3"/>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" s="2"/>
       <c r="B211" s="2"/>
-      <c r="C211" s="17"/>
+      <c r="C211" s="3"/>
+      <c r="D211" s="3"/>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" s="2"/>
       <c r="B212" s="2"/>
-      <c r="C212" s="17"/>
+      <c r="C212" s="3"/>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" s="2"/>
       <c r="B213" s="2"/>
-      <c r="C213" s="17"/>
+      <c r="C213" s="3"/>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" s="2"/>
       <c r="B214" s="2"/>
-      <c r="C214" s="17"/>
+      <c r="C214" s="3"/>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" s="2"/>
       <c r="B215" s="2"/>
-      <c r="C215" s="17"/>
+      <c r="C215" s="3"/>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" s="2"/>
       <c r="B216" s="2"/>
-      <c r="C216" s="17"/>
+      <c r="C216" s="3"/>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" s="2"/>
       <c r="B217" s="2"/>
-      <c r="C217" s="17"/>
+      <c r="C217" s="3"/>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" s="2"/>
       <c r="B218" s="2"/>
-      <c r="C218" s="17"/>
+      <c r="C218" s="3"/>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" s="2"/>
       <c r="B219" s="2"/>
-      <c r="C219" s="17"/>
+      <c r="C219" s="3"/>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" s="2"/>
       <c r="B220" s="2"/>
-      <c r="C220" s="17"/>
+      <c r="C220" s="3"/>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" s="2"/>
       <c r="B221" s="2"/>
-      <c r="C221" s="17"/>
+      <c r="C221" s="3"/>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" s="2"/>
       <c r="B222" s="2"/>
-      <c r="C222" s="17"/>
+      <c r="C222" s="3"/>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" s="2"/>
       <c r="B223" s="2"/>
-      <c r="C223" s="17"/>
+      <c r="C223" s="3"/>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" s="2"/>
       <c r="B224" s="2"/>
-      <c r="C224" s="17"/>
+      <c r="C224" s="3"/>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" s="2"/>
       <c r="B225" s="2"/>
-      <c r="C225" s="17"/>
+      <c r="C225" s="3"/>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" s="2"/>
       <c r="B226" s="2"/>
-      <c r="C226" s="17"/>
+      <c r="C226" s="3"/>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" s="2"/>
       <c r="B227" s="2"/>
-      <c r="C227" s="17"/>
+      <c r="C227" s="3"/>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" s="2"/>
       <c r="B228" s="2"/>
-      <c r="C228" s="17"/>
+      <c r="C228" s="3"/>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" s="2"/>
       <c r="B229" s="2"/>
-      <c r="C229" s="17"/>
+      <c r="C229" s="3"/>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" s="2"/>
       <c r="B230" s="2"/>
-      <c r="C230" s="17"/>
+      <c r="C230" s="3"/>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" s="2"/>
       <c r="B231" s="2"/>
-      <c r="C231" s="17"/>
+      <c r="C231" s="3"/>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" s="2"/>
       <c r="B232" s="2"/>
-      <c r="C232" s="17"/>
+      <c r="C232" s="3"/>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" s="2"/>
       <c r="B233" s="2"/>
+      <c r="C233" s="3"/>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A234" s="2"/>
+      <c r="B234" s="2"/>
+      <c r="C234" s="3"/>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A235" s="2"/>
+      <c r="B235" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{E725EB1C-4FEF-4B5C-9A88-AB23B85394CA}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>